<commit_message>
Bug Fix  - Update variables
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/90_VisualModeling_Page/WeightedModelWoe/90_LibFormula_WeightedModelWoe.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/90_VisualModeling_Page/WeightedModelWoe/90_LibFormula_WeightedModelWoe.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17329"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="31">
   <si>
     <t>Action</t>
   </si>
@@ -194,11 +194,17 @@
   <si>
     <t>deleteLink_onClick</t>
   </si>
+  <si>
+    <t>updateVariables</t>
+  </si>
+  <si>
+    <t>String, String</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -323,7 +329,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="1026" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -366,7 +378,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 2"/>
+        <xdr:cNvPr id="2" name="AutoShape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -419,7 +437,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2052" name="_xssf_cell_comment" hidden="1"/>
+        <xdr:cNvPr id="2052" name="_xssf_cell_comment" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -462,7 +486,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="AutoShape 4"/>
+        <xdr:cNvPr id="2" name="AutoShape 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -844,10 +874,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -1073,6 +1103,23 @@
       </c>
       <c r="F12" s="5" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1123,21 +1170,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100A0528662C946464F888B6D4F751B664E" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="7eb8da2da6b7d5c53beb1ead2cce6035">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b076ddd7a9ae18a4618df1e20c90f69">
     <xsd:element name="properties">
@@ -1251,10 +1283,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1275,17 +1330,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{18766838-C093-4689-97F5-C7603AB3A608}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3BDBC09D-8C85-4E54-AA93-52829A2ABEB7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>